<commit_message>
More properties written to results.xlsx
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -34,21 +34,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="38">
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>32768</t>
+  </si>
+  <si>
+    <t>464.0</t>
+  </si>
+  <si>
+    <t>32800</t>
+  </si>
+  <si>
+    <t>4.433</t>
+  </si>
+  <si>
+    <t>0.275390625</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>OX</t>
+  </si>
+  <si>
+    <t>SwapBest</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>SwapBestII</t>
+  </si>
+  <si>
+    <t>476.0</t>
+  </si>
+  <si>
+    <t>5.425</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>SwapFirstII</t>
+  </si>
+  <si>
+    <t>460.0</t>
+  </si>
+  <si>
+    <t>5.832</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>SwapRandom</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>6.581</t>
+  </si>
   <si>
     <t>PMX</t>
   </si>
   <si>
-    <t>465</t>
-  </si>
-  <si>
-    <t>Local Search</t>
-  </si>
-  <si>
-    <t>780</t>
-  </si>
-  <si>
-    <t>444.0</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>3.77</t>
+  </si>
+  <si>
+    <t>458.0</t>
+  </si>
+  <si>
+    <t>4.849</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>462.0</t>
+  </si>
+  <si>
+    <t>5.182</t>
+  </si>
+  <si>
+    <t>470.0</t>
+  </si>
+  <si>
+    <t>6.479</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>456.0</t>
+  </si>
+  <si>
+    <t>1.787</t>
+  </si>
+  <si>
+    <t>450.0</t>
+  </si>
+  <si>
+    <t>1.41</t>
   </si>
 </sst>
 </file>
@@ -420,33 +519,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str" s="0">
-        <v>Algorithm</v>
+        <v># Birds</v>
       </c>
       <c r="B1" t="str" s="0">
-        <v>Cost</v>
+        <v># Neighbours</v>
+      </c>
+      <c r="C1" t="str" s="0">
+        <v>Overlap Factor</v>
+      </c>
+      <c r="D1" t="str" s="0">
+        <v># Iterations</v>
+      </c>
+      <c r="E1" t="str" s="0">
+        <v>Final Cost</v>
+      </c>
+      <c r="F1" t="str" s="0">
+        <v># Neighbours Created</v>
+      </c>
+      <c r="G1" t="str" s="0">
+        <v>Time</v>
+      </c>
+      <c r="H1" t="str" s="0">
+        <v>Density</v>
+      </c>
+      <c r="I1" t="str" s="0">
+        <v># Types</v>
+      </c>
+      <c r="J1" t="str" s="0">
+        <v>Crossover</v>
+      </c>
+      <c r="K1" t="str" s="0">
+        <v>Mutation</v>
+      </c>
+      <c r="L1" t="str" s="0">
+        <v>Mutation Intensity</v>
+      </c>
+      <c r="M1" t="str" s="0">
+        <v>Local Search</v>
+      </c>
+      <c r="N1" t="str" s="0">
+        <v>Depth of Local Search</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>1</v>
+      <c r="A2" t="str" s="0">
+        <v>51</v>
+      </c>
+      <c r="B2" t="str" s="0">
+        <v>5</v>
+      </c>
+      <c r="C2" t="str" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str" s="0">
+        <v>32768</v>
+      </c>
+      <c r="E2" t="str" s="0">
+        <v>454.0</v>
+      </c>
+      <c r="F2" t="str" s="0">
+        <v>32800</v>
+      </c>
+      <c r="G2" t="str" s="0">
+        <v>6.496</v>
+      </c>
+      <c r="H2" t="str" s="0">
+        <v>0.275390625</v>
+      </c>
+      <c r="I2" t="str" s="0">
+        <v>32</v>
+      </c>
+      <c r="J2" t="str" s="0">
+        <v>PMX</v>
+      </c>
+      <c r="K2" t="str" s="0">
+        <v>SwapBest</v>
+      </c>
+      <c r="L2" t="str" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="M2" t="str" s="0">
+        <v>SwapFirstII</v>
+      </c>
+      <c r="N2" t="str" s="0">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>3</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -454,20 +661,400 @@
         <v>0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="D5" t="s" s="0">
         <v>3</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M8" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="L10" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="M11" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N11" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="L12" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="M12" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update excel for none counter
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emir/MMBO-Algorithm-QAP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1F5CFB-894F-E240-94D0-45AEDCAA630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D21F91D-FD2E-194B-9F79-19A7C6170255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t># Birds</t>
   </si>
@@ -73,6 +73,9 @@
     <t>U_CX_COUNTER</t>
   </si>
   <si>
+    <t>U_NONE_COUNTER</t>
+  </si>
+  <si>
     <t>U_SWAPRANDOM_COUNTER</t>
   </si>
   <si>
@@ -118,74 +121,70 @@
     <t>U_DLS_5_COUNTER</t>
   </si>
   <si>
-    <t>A_PMX_COANTER</t>
-  </si>
-  <si>
-    <t>A_OX_COANTER</t>
-  </si>
-  <si>
-    <t>A_CX_COANTER</t>
-  </si>
-  <si>
-    <t>A_SWAPRANDOM_COANTER</t>
-  </si>
-  <si>
-    <t>A_SWAPBEST_COANTER</t>
-  </si>
-  <si>
-    <t>A_SCRAMBLE_COANTER</t>
-  </si>
-  <si>
-    <t>A_SFII_COANTER</t>
-  </si>
-  <si>
-    <t>A_SBII_COANTER</t>
-  </si>
-  <si>
-    <t>A_MI_0.2_COANTER</t>
-  </si>
-  <si>
-    <t>A_MI_0.4_COANTER</t>
-  </si>
-  <si>
-    <t>A_MI_0.6_COANTER</t>
-  </si>
-  <si>
-    <t>A_MI_0.8_COANTER</t>
-  </si>
-  <si>
-    <t>A_MI_1_COANTER</t>
-  </si>
-  <si>
-    <t>A_DLS_1_COANTER</t>
-  </si>
-  <si>
-    <t>A_DLS_2_COANTER</t>
-  </si>
-  <si>
-    <t>A_DLS_3_COANTER</t>
-  </si>
-  <si>
-    <t>A_DLS_4_COANTER</t>
-  </si>
-  <si>
-    <t>A_DLS_5_COANTER</t>
+    <t>A_NONE_COUNTER</t>
+  </si>
+  <si>
+    <t>A_PMX_COUNTER</t>
+  </si>
+  <si>
+    <t>A_OX_COUNTER</t>
+  </si>
+  <si>
+    <t>A_CX_COUNTER</t>
+  </si>
+  <si>
+    <t>A_SWAPRANDOM_COUNTER</t>
+  </si>
+  <si>
+    <t>A_SWAPBEST_COUNTER</t>
+  </si>
+  <si>
+    <t>A_SCRAMBLE_COUNTER</t>
+  </si>
+  <si>
+    <t>A_SFII_COUNTER</t>
+  </si>
+  <si>
+    <t>A_SBII_COUNTER</t>
+  </si>
+  <si>
+    <t>A_MI_0.2_COUNTER</t>
+  </si>
+  <si>
+    <t>A_MI_0.4_COUNTER</t>
+  </si>
+  <si>
+    <t>A_MI_0.6_COUNTER</t>
+  </si>
+  <si>
+    <t>A_MI_0.8_COUNTER</t>
+  </si>
+  <si>
+    <t>A_MI_1_COUNTER</t>
+  </si>
+  <si>
+    <t>A_DLS_1_COUNTER</t>
+  </si>
+  <si>
+    <t>A_DLS_2_COUNTER</t>
+  </si>
+  <si>
+    <t>A_DLS_3_COUNTER</t>
+  </si>
+  <si>
+    <t>A_DLS_4_COUNTER</t>
+  </si>
+  <si>
+    <t>A_DLS_5_COUNTER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -212,9 +211,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,167 +552,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX1"/>
+  <dimension ref="A1:AZ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="A2:N12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.33203125" customWidth="1"/>
+    <col min="38" max="38" width="25.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" t="s">
         <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:AG1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>